<commit_message>
Improved code inside Login test page
</commit_message>
<xml_diff>
--- a/src/test/java/TestData.xlsx
+++ b/src/test/java/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Private\Desktop\FinalProject\src\test\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97FE4BA-A725-4881-A349-C4171230CE50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AED3A05-53A3-4880-8F2E-1A2F07CAF3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>valid username</t>
   </si>
@@ -43,9 +43,6 @@
     <t>sada123</t>
   </si>
   <si>
-    <t>sada</t>
-  </si>
-  <si>
     <t>locked_out_user</t>
   </si>
   <si>
@@ -77,13 +74,25 @@
   </si>
   <si>
     <t>41ada21000</t>
+  </si>
+  <si>
+    <t>valid password / invalid username</t>
+  </si>
+  <si>
+    <t>valid username / invalid password</t>
+  </si>
+  <si>
+    <t>asdds</t>
+  </si>
+  <si>
+    <t>sad11111111</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -100,6 +109,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -123,7 +139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -170,11 +186,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -187,6 +229,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,10 +454,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:E7"/>
+  <dimension ref="B1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -416,9 +465,10 @@
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
     <col min="3" max="3" width="25.21875" customWidth="1"/>
     <col min="4" max="5" width="25.33203125" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,7 +482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
@@ -443,70 +493,77 @@
         <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4">
-        <v>123</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
-        <v>12</v>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="4">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>14</v>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="4">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
-        <v>16</v>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>